<commit_message>
Your commit message here
</commit_message>
<xml_diff>
--- a/internal data/external data sources.xlsx
+++ b/internal data/external data sources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcbtkov_ucl_ac_uk/Documents/MSci Bahler lab/S.-Pombe-biofilm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/91277b806043e344/MSci Bahler lab/S.-Pombe-MLPs - Github/internal data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{306732B4-4BF7-7F46-B5F7-D97A7D54F9A0}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D32B8F3B-62D2-554D-A6F5-2542CCAA6353}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="740" windowWidth="23960" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>Author</t>
   </si>
@@ -50,18 +50,12 @@
     <t>Accessed from</t>
   </si>
   <si>
-    <t>Clement-Ziza et al.</t>
-  </si>
-  <si>
     <t>RNA-seq of segregants grown on EMM</t>
   </si>
   <si>
     <t>Raw count matrix</t>
   </si>
   <si>
-    <t>DEseq</t>
-  </si>
-  <si>
     <t>Supplementary dataset S4</t>
   </si>
   <si>
@@ -77,18 +71,12 @@
     <t>ENA: ERX007392 and ERX007395</t>
   </si>
   <si>
-    <t>Rubio et al.</t>
-  </si>
-  <si>
     <t>RNA-seq data in environmental stresses</t>
   </si>
   <si>
     <t>Supplementary files</t>
   </si>
   <si>
-    <t>Jeffares et al.</t>
-  </si>
-  <si>
     <t>Short variants in wild isolates</t>
   </si>
   <si>
@@ -98,9 +86,6 @@
     <t>Figshare associate with publication</t>
   </si>
   <si>
-    <t>Atkinson et al.</t>
-  </si>
-  <si>
     <t>RNA-seq in various conditions (including EMM and YES)</t>
   </si>
   <si>
@@ -110,27 +95,18 @@
     <t>Supplementary table 3.</t>
   </si>
   <si>
-    <t>Kwon et al.</t>
-  </si>
-  <si>
     <t>Processed list of hits</t>
   </si>
   <si>
     <t>Processed list of fold-change values</t>
   </si>
   <si>
-    <t>Linder et al.</t>
-  </si>
-  <si>
     <t>Microarray data on Mediator deletion strains grown on EMM</t>
   </si>
   <si>
     <t>Processed matrix</t>
   </si>
   <si>
-    <t>Szilagyi et al.</t>
-  </si>
-  <si>
     <t>Raw .CEL files</t>
   </si>
   <si>
@@ -138,9 +114,6 @@
   </si>
   <si>
     <t>GEO: GSE31642</t>
-  </si>
-  <si>
-    <t>Garg et al.</t>
   </si>
   <si>
     <t>Processed fold-change matrix</t>
@@ -280,6 +253,45 @@
   </si>
   <si>
     <t>Processed list of targets</t>
+  </si>
+  <si>
+    <t>Clement-Ziza et al. (2014)</t>
+  </si>
+  <si>
+    <t>RNA-seq of lab strain grown in Phosphate-minus media</t>
+  </si>
+  <si>
+    <t>Processed DEseq comparison between timepoints</t>
+  </si>
+  <si>
+    <t>DESeq</t>
+  </si>
+  <si>
+    <t>GEO: GSE217953</t>
+  </si>
+  <si>
+    <t>Garg et al. (2023)</t>
+  </si>
+  <si>
+    <t>Kwon et al. (2012)</t>
+  </si>
+  <si>
+    <t>Linder et al. (2008)</t>
+  </si>
+  <si>
+    <t>Szilagyi et al. (2012)</t>
+  </si>
+  <si>
+    <t>Garg et al. (2015)</t>
+  </si>
+  <si>
+    <t>Rubio et al. (2021)</t>
+  </si>
+  <si>
+    <t>Jeffares et al. (2015)</t>
+  </si>
+  <si>
+    <t>Atkinson et al. (2018)</t>
   </si>
 </sst>
 </file>
@@ -317,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -340,14 +352,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -364,10 +389,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -667,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -683,207 +704,224 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>